<commit_message>
Merging of VWAP data and brand data
</commit_message>
<xml_diff>
--- a/data/brand_Kantar.xlsx
+++ b/data/brand_Kantar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johannaschulz/Documents/GitHub/EconometricAnalysis-BrandCrisisModeration-DAX30/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF90C6EE-0227-4D49-9CDB-8664335EA234}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BAD8D6E-4D20-C344-9234-3337341404A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-34000" yWindow="-640" windowWidth="27640" windowHeight="16760" xr2:uid="{EC95F2B1-67CE-DF42-9465-0AD532F8D67B}"/>
   </bookViews>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="117">
   <si>
     <t>Adidas AG (former: -Solomon)</t>
   </si>
@@ -394,29 +394,6 @@
     <t>Cars, Auto Manufacturers</t>
   </si>
   <si>
-    <r>
-      <t>VOW3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>.F</t>
-    </r>
-  </si>
-  <si>
     <t>Audi</t>
   </si>
   <si>
@@ -463,6 +440,9 @@
   </si>
   <si>
     <t>VOW3.F</t>
+  </si>
+  <si>
+    <t>LIN.F</t>
   </si>
 </sst>
 </file>
@@ -912,36 +892,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{981D7B6B-1E1B-354E-BEBE-35F7FFA9C602}">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:8" ht="42" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="10" t="s">
         <v>114</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="42" x14ac:dyDescent="0.2">
@@ -1208,7 +1188,7 @@
         <v>41</v>
       </c>
       <c r="G12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -1234,7 +1214,7 @@
         <v>41</v>
       </c>
       <c r="G13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -1430,7 +1410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" ht="28" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>72</v>
       </c>
@@ -1439,9 +1419,15 @@
       <c r="D22" s="2">
         <v>0</v>
       </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
+      <c r="E22" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>116</v>
+      </c>
       <c r="H22">
         <v>0</v>
       </c>
@@ -1636,7 +1622,7 @@
         <v>3</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="H30">
         <v>1</v>
@@ -1647,7 +1633,7 @@
         <v>97</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C31" s="2">
         <v>7</v>
@@ -1662,7 +1648,7 @@
         <v>3</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="H31">
         <v>1</v>
@@ -1673,7 +1659,7 @@
         <v>97</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C32" s="2">
         <v>16</v>
@@ -1688,7 +1674,7 @@
         <v>3</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H32">
         <v>1</v>
@@ -1696,7 +1682,7 @@
     </row>
     <row r="33" spans="1:8" ht="28" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -1704,13 +1690,13 @@
         <v>0</v>
       </c>
       <c r="E33" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F33" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="G33" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>106</v>
       </c>
       <c r="H33">
         <v>0</v>

</xml_diff>